<commit_message>
Content for Pet Shu added!
Former-commit-id: 387efbc7c35c365823a000bd1d9f77da825a8e1c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Pets.xlsx
+++ b/Docs/Content/HungryDragonContent_Pets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="632">
   <si>
     <t>[sku]</t>
   </si>
@@ -1917,6 +1917,30 @@
   </si>
   <si>
     <t>Mexican_62_</t>
+  </si>
+  <si>
+    <t>pet_75</t>
+  </si>
+  <si>
+    <t>PF_PetShu_75</t>
+  </si>
+  <si>
+    <t>PF_PetShuMenu_75</t>
+  </si>
+  <si>
+    <t>pet_shu_75</t>
+  </si>
+  <si>
+    <t>TID_PET_75_NAME</t>
+  </si>
+  <si>
+    <t>TID_PET_75_DESC</t>
+  </si>
+  <si>
+    <t>coin_throw</t>
+  </si>
+  <si>
+    <t>Shu_75_coin_throw</t>
   </si>
 </sst>
 </file>
@@ -3248,8 +3272,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="petDefinitions" displayName="petDefinitions" ref="B4:T79" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="B4:T79"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="petDefinitions" displayName="petDefinitions" ref="B4:T80" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="B4:T80"/>
   <sortState ref="B5:T77">
     <sortCondition ref="D4:D77"/>
   </sortState>
@@ -3283,8 +3307,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="petCategoryDefinitions" displayName="petCategoryDefinitions" ref="B93:F100" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B93:F100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="petCategoryDefinitions" displayName="petCategoryDefinitions" ref="B94:F101" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B94:F101"/>
   <sortState ref="B80:F86">
     <sortCondition ref="D77:D84"/>
   </sortState>
@@ -3565,10 +3589,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:T100"/>
+  <dimension ref="B1:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3587,7 +3611,7 @@
     <col min="14" max="14" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23" customWidth="1"/>
     <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="41.85546875" bestFit="1" customWidth="1"/>
@@ -7743,9 +7767,7 @@
       <c r="J78" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="K78" s="25" t="s">
-        <v>477</v>
-      </c>
+      <c r="K78" s="25"/>
       <c r="L78" s="25"/>
       <c r="M78" s="8" t="s">
         <v>478</v>
@@ -7829,107 +7851,125 @@
         <v>511</v>
       </c>
     </row>
-    <row r="80" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="81" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B81" s="1" t="s">
+    <row r="80" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B80" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="29" t="s">
+        <v>624</v>
+      </c>
+      <c r="D80" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="25">
+        <v>22</v>
+      </c>
+      <c r="G80" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H80" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I80" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J80" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K80" s="25" t="s">
+        <v>477</v>
+      </c>
+      <c r="L80" s="25"/>
+      <c r="M80" s="8" t="s">
+        <v>625</v>
+      </c>
+      <c r="N80" s="8" t="s">
+        <v>626</v>
+      </c>
+      <c r="O80" s="31" t="s">
+        <v>627</v>
+      </c>
+      <c r="P80" s="15" t="s">
+        <v>630</v>
+      </c>
+      <c r="Q80" s="11" t="s">
+        <v>628</v>
+      </c>
+      <c r="R80" s="16" t="s">
+        <v>629</v>
+      </c>
+      <c r="S80" s="11">
+        <v>75</v>
+      </c>
+      <c r="T80" s="25" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="81" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B82" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
-      <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
-      <c r="N81" s="1"/>
-      <c r="O81" s="1"/>
-      <c r="P81" s="1"/>
-      <c r="Q81" s="1"/>
-    </row>
-    <row r="83" spans="2:17" ht="135" x14ac:dyDescent="0.25">
-      <c r="B83" s="20" t="s">
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+    </row>
+    <row r="84" spans="2:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="B84" s="20" t="s">
         <v>371</v>
       </c>
-      <c r="C83" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D83" s="21" t="s">
+      <c r="C84" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="21" t="s">
         <v>372</v>
       </c>
-      <c r="E83" s="21" t="s">
+      <c r="E84" s="21" t="s">
         <v>373</v>
       </c>
-      <c r="F83" s="21" t="s">
+      <c r="F84" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="G83" s="21" t="s">
+      <c r="G84" s="21" t="s">
         <v>375</v>
       </c>
-      <c r="H83" s="21" t="s">
+      <c r="H84" s="21" t="s">
         <v>376</v>
       </c>
-      <c r="I83" s="22" t="s">
+      <c r="I84" s="22" t="s">
         <v>377</v>
       </c>
-      <c r="J83" s="22" t="s">
+      <c r="J84" s="22" t="s">
         <v>378</v>
       </c>
-      <c r="K83" s="22"/>
-      <c r="L83" s="22"/>
-      <c r="M83" s="22" t="s">
+      <c r="K84" s="22"/>
+      <c r="L84" s="22"/>
+      <c r="M84" s="22" t="s">
         <v>379</v>
       </c>
-      <c r="N83" s="22" t="s">
+      <c r="N84" s="22" t="s">
         <v>380</v>
       </c>
-      <c r="O83" s="22" t="s">
+      <c r="O84" s="22" t="s">
         <v>381</v>
       </c>
-      <c r="P83" s="22" t="s">
+      <c r="P84" s="22" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="84" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B84" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C84" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D84" s="25">
-        <v>1.3</v>
-      </c>
-      <c r="E84" s="25">
-        <v>4</v>
-      </c>
-      <c r="F84" s="25">
-        <v>1.3</v>
-      </c>
-      <c r="G84" s="25">
-        <v>1000</v>
-      </c>
-      <c r="H84" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="I84" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="J84" s="8"/>
-      <c r="K84" s="8"/>
-      <c r="L84" s="8"/>
-      <c r="M84" s="8"/>
-      <c r="N84" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="O84" s="8">
-        <v>4</v>
-      </c>
-      <c r="P84" s="8">
-        <v>2</v>
       </c>
     </row>
     <row r="85" spans="2:17" x14ac:dyDescent="0.25">
@@ -7937,7 +7977,7 @@
         <v>2</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>383</v>
+        <v>11</v>
       </c>
       <c r="D85" s="25">
         <v>1.3</v>
@@ -7952,14 +7992,12 @@
         <v>1000</v>
       </c>
       <c r="H85" s="25">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="I85" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="J85" s="8" t="s">
-        <v>384</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="J85" s="8"/>
       <c r="K85" s="8"/>
       <c r="L85" s="8"/>
       <c r="M85" s="8"/>
@@ -7974,11 +8012,11 @@
       </c>
     </row>
     <row r="86" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B86" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C86" s="27" t="s">
-        <v>385</v>
+      <c r="B86" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="24" t="s">
+        <v>383</v>
       </c>
       <c r="D86" s="25">
         <v>1.3</v>
@@ -7999,7 +8037,7 @@
         <v>0.5</v>
       </c>
       <c r="J86" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K86" s="8"/>
       <c r="L86" s="8"/>
@@ -8019,7 +8057,7 @@
         <v>2</v>
       </c>
       <c r="C87" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D87" s="25">
         <v>1.3</v>
@@ -8034,17 +8072,17 @@
         <v>1000</v>
       </c>
       <c r="H87" s="25">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="I87" s="8">
-        <v>10</v>
-      </c>
-      <c r="J87" s="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="J87" s="8" t="s">
+        <v>386</v>
+      </c>
       <c r="K87" s="8"/>
       <c r="L87" s="8"/>
-      <c r="M87" s="8" t="s">
-        <v>386</v>
-      </c>
+      <c r="M87" s="8"/>
       <c r="N87" s="8" t="b">
         <v>0</v>
       </c>
@@ -8052,7 +8090,7 @@
         <v>4</v>
       </c>
       <c r="P87" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="2:17" x14ac:dyDescent="0.25">
@@ -8060,7 +8098,7 @@
         <v>2</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>45</v>
+        <v>387</v>
       </c>
       <c r="D88" s="25">
         <v>1.3</v>
@@ -8069,17 +8107,23 @@
         <v>4</v>
       </c>
       <c r="F88" s="25">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="G88" s="25">
         <v>1000</v>
       </c>
-      <c r="H88" s="25"/>
-      <c r="I88" s="8"/>
+      <c r="H88" s="25">
+        <v>10</v>
+      </c>
+      <c r="I88" s="8">
+        <v>10</v>
+      </c>
       <c r="J88" s="8"/>
       <c r="K88" s="8"/>
       <c r="L88" s="8"/>
-      <c r="M88" s="8"/>
+      <c r="M88" s="8" t="s">
+        <v>386</v>
+      </c>
       <c r="N88" s="8" t="b">
         <v>0</v>
       </c>
@@ -8087,7 +8131,7 @@
         <v>4</v>
       </c>
       <c r="P88" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="2:17" x14ac:dyDescent="0.25">
@@ -8095,7 +8139,7 @@
         <v>2</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D89" s="25">
         <v>1.3</v>
@@ -8104,20 +8148,14 @@
         <v>4</v>
       </c>
       <c r="F89" s="25">
-        <v>1.3</v>
+        <v>3</v>
       </c>
       <c r="G89" s="25">
         <v>1000</v>
       </c>
-      <c r="H89" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="I89" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="J89" s="8" t="s">
-        <v>388</v>
-      </c>
+      <c r="H89" s="25"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
       <c r="K89" s="8"/>
       <c r="L89" s="8"/>
       <c r="M89" s="8"/>
@@ -8131,94 +8169,118 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="91" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B91" s="1" t="s">
+    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B90" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D90" s="25">
+        <v>1.3</v>
+      </c>
+      <c r="E90" s="25">
+        <v>4</v>
+      </c>
+      <c r="F90" s="25">
+        <v>1.3</v>
+      </c>
+      <c r="G90" s="25">
+        <v>1000</v>
+      </c>
+      <c r="H90" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="I90" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="J90" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="K90" s="8"/>
+      <c r="L90" s="8"/>
+      <c r="M90" s="8"/>
+      <c r="N90" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="O90" s="8">
+        <v>4</v>
+      </c>
+      <c r="P90" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B92" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
-      <c r="J91" s="1"/>
-      <c r="K91" s="1"/>
-      <c r="L91" s="1"/>
-      <c r="M91" s="1"/>
-      <c r="N91" s="1"/>
-    </row>
-    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-    </row>
-    <row r="93" spans="2:17" ht="123" x14ac:dyDescent="0.25">
-      <c r="B93" s="3" t="s">
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+    </row>
+    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+    </row>
+    <row r="94" spans="2:17" ht="123" x14ac:dyDescent="0.25">
+      <c r="B94" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="C93" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D93" s="9" t="s">
+      <c r="C94" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E93" s="5" t="s">
+      <c r="E94" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F93" s="6" t="s">
+      <c r="F94" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B94" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C94" s="24" t="s">
+    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B95" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D94" s="13">
-        <v>0</v>
-      </c>
-      <c r="E94" s="14" t="s">
+      <c r="D95" s="13">
+        <v>0</v>
+      </c>
+      <c r="E95" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F94" s="28" t="s">
+      <c r="F95" s="28" t="s">
         <v>391</v>
-      </c>
-    </row>
-    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B95" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C95" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D95" s="18">
-        <v>1</v>
-      </c>
-      <c r="E95" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F95" s="28" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="96" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B96" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C96" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D96" s="13">
-        <v>2</v>
-      </c>
-      <c r="E96" s="14" t="s">
-        <v>30</v>
+      <c r="C96" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D96" s="18">
+        <v>1</v>
+      </c>
+      <c r="E96" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="F96" s="28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
@@ -8226,16 +8288,16 @@
         <v>2</v>
       </c>
       <c r="C97" s="24" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D97" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E97" s="14" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="F97" s="28" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
@@ -8243,16 +8305,16 @@
         <v>2</v>
       </c>
       <c r="C98" s="24" t="s">
-        <v>134</v>
+        <v>4</v>
       </c>
       <c r="D98" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E98" s="14" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="F98" s="28" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
@@ -8260,16 +8322,16 @@
         <v>2</v>
       </c>
       <c r="C99" s="24" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D99" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E99" s="14" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F99" s="28" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
@@ -8277,22 +8339,39 @@
         <v>2</v>
       </c>
       <c r="C100" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D100" s="13">
+        <v>5</v>
+      </c>
+      <c r="E100" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F100" s="28" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D100" s="13">
+      <c r="D101" s="13">
         <v>6</v>
       </c>
-      <c r="E100" s="14" t="s">
+      <c r="E101" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F100" s="28" t="s">
+      <c r="F101" s="28" t="s">
         <v>397</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D84:H89 F5:F23 F25:F26 F28:F79 G5:L79"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E5:E79">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D85:H90 F5:F23 F25:F26 F28:F80 G5:L80"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E5:E80">
       <formula1>INDIRECT("petCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
old power up sku "coins" now is "coins_better"
Former-commit-id: 7211791b6f66b83c71fa3b38dc651a77637af84f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Pets.xlsx
+++ b/Docs/Content/HungryDragonContent_Pets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="pet" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>icon_score</t>
-  </si>
-  <si>
-    <t>coins</t>
   </si>
   <si>
     <t>dive</t>
@@ -1941,6 +1938,9 @@
   </si>
   <si>
     <t>Shu_75_coin_throw</t>
+  </si>
+  <si>
+    <t>coins_better</t>
   </si>
 </sst>
 </file>
@@ -3591,8 +3591,8 @@
   </sheetPr>
   <dimension ref="B1:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3620,7 +3620,7 @@
     <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3641,61 +3641,61 @@
     </row>
     <row r="4" spans="2:20" ht="104.25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>401</v>
-      </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="P4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
@@ -3703,10 +3703,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>4</v>
@@ -3729,28 +3729,28 @@
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
       <c r="M5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="P5" s="15" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q5" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="P5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>80</v>
-      </c>
       <c r="R5" s="11" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S5" s="11">
         <v>0</v>
       </c>
       <c r="T5" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
@@ -3758,10 +3758,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>4</v>
@@ -3784,28 +3784,28 @@
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
       <c r="M6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="P6" s="15" t="s">
         <v>4</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="S6" s="16">
         <v>1</v>
       </c>
       <c r="T6" s="25" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
@@ -3813,13 +3813,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="25">
         <v>2</v>
@@ -3839,28 +3839,28 @@
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
       <c r="M7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="P7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="P7" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q7" s="11" t="s">
-        <v>91</v>
-      </c>
       <c r="R7" s="16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="S7" s="11">
         <v>2</v>
       </c>
       <c r="T7" s="25" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
@@ -3868,10 +3868,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>4</v>
@@ -3894,28 +3894,28 @@
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
       <c r="M8" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="N8" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="O8" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="P8" s="15" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q8" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="P8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="R8" s="11" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="S8" s="16">
         <v>3</v>
       </c>
       <c r="T8" s="25" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
@@ -3923,13 +3923,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="25">
         <v>3</v>
@@ -3949,28 +3949,28 @@
       <c r="K9" s="25"/>
       <c r="L9" s="25"/>
       <c r="M9" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="N9" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N9" s="8" t="s">
+      <c r="O9" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="O9" s="31" t="s">
+      <c r="P9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="P9" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q9" s="11" t="s">
-        <v>101</v>
-      </c>
       <c r="R9" s="16" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S9" s="11">
         <v>4</v>
       </c>
       <c r="T9" s="25" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -3978,10 +3978,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>4</v>
@@ -4004,28 +4004,28 @@
       <c r="K10" s="37"/>
       <c r="L10" s="37"/>
       <c r="M10" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="N10" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="N10" s="39" t="s">
+      <c r="O10" s="39" t="s">
         <v>104</v>
-      </c>
-      <c r="O10" s="39" t="s">
-        <v>105</v>
       </c>
       <c r="P10" s="36" t="s">
         <v>4</v>
       </c>
       <c r="Q10" s="35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R10" s="35" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="S10" s="35">
         <v>5</v>
       </c>
       <c r="T10" s="37" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
@@ -4033,13 +4033,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="37">
         <v>4</v>
@@ -4059,28 +4059,28 @@
       <c r="K11" s="37"/>
       <c r="L11" s="37"/>
       <c r="M11" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="N11" s="39" t="s">
+      <c r="O11" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="O11" s="39" t="s">
+      <c r="P11" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q11" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="P11" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q11" s="35" t="s">
-        <v>111</v>
-      </c>
       <c r="R11" s="35" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="S11" s="35">
         <v>6</v>
       </c>
       <c r="T11" s="37" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
@@ -4088,13 +4088,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="37">
         <v>0</v>
@@ -4114,28 +4114,28 @@
       <c r="K12" s="37"/>
       <c r="L12" s="37"/>
       <c r="M12" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="N12" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="N12" s="39" t="s">
+      <c r="O12" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="O12" s="39" t="s">
+      <c r="P12" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="P12" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="35" t="s">
-        <v>116</v>
-      </c>
       <c r="R12" s="35" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="S12" s="35">
         <v>7</v>
       </c>
       <c r="T12" s="37" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
@@ -4143,13 +4143,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>117</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>118</v>
       </c>
       <c r="F13" s="37">
         <v>0</v>
@@ -4169,28 +4169,28 @@
       <c r="K13" s="37"/>
       <c r="L13" s="37"/>
       <c r="M13" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="N13" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="N13" s="39" t="s">
+      <c r="O13" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="O13" s="39" t="s">
+      <c r="P13" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q13" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="P13" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q13" s="35" t="s">
-        <v>122</v>
-      </c>
       <c r="R13" s="35" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="S13" s="35">
         <v>8</v>
       </c>
       <c r="T13" s="37" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
@@ -4198,13 +4198,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="37">
         <v>0</v>
@@ -4224,28 +4224,28 @@
       <c r="K14" s="37"/>
       <c r="L14" s="37"/>
       <c r="M14" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="N14" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="N14" s="40" t="s">
+      <c r="O14" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="O14" s="39" t="s">
+      <c r="P14" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q14" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="P14" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q14" s="35" t="s">
-        <v>127</v>
-      </c>
       <c r="R14" s="35" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="S14" s="35">
         <v>9</v>
       </c>
       <c r="T14" s="37" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
@@ -4253,13 +4253,13 @@
         <v>2</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="25">
         <v>1</v>
@@ -4279,28 +4279,28 @@
       <c r="K15" s="25"/>
       <c r="L15" s="25"/>
       <c r="M15" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="N15" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="N15" s="8" t="s">
+      <c r="O15" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="O15" s="8" t="s">
+      <c r="P15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="P15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q15" s="11" t="s">
-        <v>132</v>
-      </c>
       <c r="R15" s="11" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="S15" s="11">
         <v>10</v>
       </c>
       <c r="T15" s="25" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
@@ -4308,13 +4308,13 @@
         <v>2</v>
       </c>
       <c r="C16" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="25" t="s">
         <v>133</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>134</v>
       </c>
       <c r="F16" s="25">
         <v>0</v>
@@ -4334,28 +4334,28 @@
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
       <c r="M16" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="N16" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="N16" s="8" t="s">
+      <c r="O16" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="O16" s="8" t="s">
+      <c r="P16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="P16" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q16" s="11" t="s">
-        <v>138</v>
-      </c>
       <c r="R16" s="11" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="S16" s="16">
         <v>11</v>
       </c>
       <c r="T16" s="25" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
@@ -4363,13 +4363,13 @@
         <v>2</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F17" s="25">
         <v>1</v>
@@ -4389,28 +4389,28 @@
       <c r="K17" s="25"/>
       <c r="L17" s="25"/>
       <c r="M17" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="N17" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="N17" s="8" t="s">
+      <c r="O17" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="O17" s="8" t="s">
+      <c r="P17" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="P17" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q17" s="11" t="s">
-        <v>148</v>
-      </c>
       <c r="R17" s="16" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="S17" s="11">
         <v>13</v>
       </c>
       <c r="T17" s="25" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
@@ -4418,10 +4418,10 @@
         <v>2</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>4</v>
@@ -4444,28 +4444,28 @@
       <c r="K18" s="25"/>
       <c r="L18" s="25"/>
       <c r="M18" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="N18" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="N18" s="8" t="s">
+      <c r="O18" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="O18" s="8" t="s">
+      <c r="P18" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q18" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="P18" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q18" s="11" t="s">
-        <v>153</v>
-      </c>
       <c r="R18" s="11" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="S18" s="16">
         <v>14</v>
       </c>
       <c r="T18" s="25" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
@@ -4473,13 +4473,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F19" s="25">
         <v>1</v>
@@ -4499,28 +4499,28 @@
       <c r="K19" s="25"/>
       <c r="L19" s="25"/>
       <c r="M19" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="N19" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="N19" s="8" t="s">
+      <c r="O19" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="O19" s="31" t="s">
+      <c r="P19" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="P19" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q19" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="R19" s="16" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="S19" s="11">
         <v>15</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
@@ -4528,13 +4528,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" s="37">
         <v>2</v>
@@ -4554,28 +4554,28 @@
       <c r="K20" s="37"/>
       <c r="L20" s="37"/>
       <c r="M20" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="N20" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="N20" s="39" t="s">
+      <c r="O20" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="O20" s="39" t="s">
+      <c r="P20" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q20" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="P20" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q20" s="35" t="s">
-        <v>163</v>
-      </c>
       <c r="R20" s="35" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="S20" s="35">
         <v>16</v>
       </c>
       <c r="T20" s="37" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
@@ -4583,13 +4583,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21" s="37">
         <v>3</v>
@@ -4609,28 +4609,28 @@
       <c r="K21" s="37"/>
       <c r="L21" s="37"/>
       <c r="M21" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="N21" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="N21" s="39" t="s">
+      <c r="O21" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="O21" s="39" t="s">
+      <c r="P21" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q21" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="P21" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q21" s="35" t="s">
-        <v>168</v>
-      </c>
       <c r="R21" s="35" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="S21" s="35">
         <v>17</v>
       </c>
       <c r="T21" s="37" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
@@ -4638,13 +4638,13 @@
         <v>2</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F22" s="37">
         <v>2</v>
@@ -4664,28 +4664,28 @@
       <c r="K22" s="37"/>
       <c r="L22" s="37"/>
       <c r="M22" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="N22" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="N22" s="39" t="s">
+      <c r="O22" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="O22" s="39" t="s">
+      <c r="P22" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q22" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="P22" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q22" s="35" t="s">
-        <v>173</v>
-      </c>
       <c r="R22" s="35" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="S22" s="35">
         <v>18</v>
       </c>
       <c r="T22" s="37" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
@@ -4693,13 +4693,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F23" s="37">
         <v>3</v>
@@ -4719,28 +4719,28 @@
       <c r="K23" s="37"/>
       <c r="L23" s="37"/>
       <c r="M23" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="N23" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="N23" s="39" t="s">
+      <c r="O23" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="O23" s="39" t="s">
+      <c r="P23" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q23" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="P23" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q23" s="35" t="s">
-        <v>178</v>
-      </c>
       <c r="R23" s="35" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="S23" s="35">
         <v>19</v>
       </c>
       <c r="T23" s="37" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
@@ -4748,13 +4748,13 @@
         <v>2</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F24" s="37">
         <v>2</v>
@@ -4774,28 +4774,28 @@
       <c r="K24" s="37"/>
       <c r="L24" s="37"/>
       <c r="M24" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="N24" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="N24" s="40" t="s">
+      <c r="O24" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="O24" s="39" t="s">
+      <c r="P24" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q24" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="P24" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q24" s="35" t="s">
-        <v>183</v>
-      </c>
       <c r="R24" s="35" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="S24" s="35">
         <v>20</v>
       </c>
       <c r="T24" s="37" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
@@ -4803,13 +4803,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F25" s="25">
         <v>3</v>
@@ -4829,28 +4829,28 @@
       <c r="K25" s="25"/>
       <c r="L25" s="25"/>
       <c r="M25" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="N25" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="N25" s="8" t="s">
+      <c r="O25" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="O25" s="8" t="s">
+      <c r="P25" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q25" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="P25" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q25" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="R25" s="11" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="S25" s="11">
         <v>21</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
@@ -4858,13 +4858,13 @@
         <v>2</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F26" s="25">
         <v>4</v>
@@ -4884,28 +4884,28 @@
       <c r="K26" s="25"/>
       <c r="L26" s="25"/>
       <c r="M26" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="N26" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="N26" s="8" t="s">
+      <c r="O26" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="O26" s="8" t="s">
+      <c r="P26" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q26" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="P26" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q26" s="11" t="s">
-        <v>193</v>
-      </c>
       <c r="R26" s="11" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="S26" s="16">
         <v>22</v>
       </c>
       <c r="T26" s="25" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
@@ -4913,13 +4913,13 @@
         <v>2</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F27" s="25">
         <v>5</v>
@@ -4939,28 +4939,28 @@
       <c r="K27" s="25"/>
       <c r="L27" s="25"/>
       <c r="M27" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="N27" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="N27" s="8" t="s">
+      <c r="O27" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="O27" s="8" t="s">
+      <c r="P27" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q27" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="P27" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q27" s="11" t="s">
-        <v>198</v>
-      </c>
       <c r="R27" s="16" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="S27" s="11">
         <v>23</v>
       </c>
       <c r="T27" s="25" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
@@ -4968,13 +4968,13 @@
         <v>2</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F28" s="25">
         <v>0</v>
@@ -4994,28 +4994,28 @@
       <c r="K28" s="25"/>
       <c r="L28" s="25"/>
       <c r="M28" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="N28" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="N28" s="8" t="s">
+      <c r="O28" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="P28" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q28" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="O28" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="P28" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q28" s="11" t="s">
-        <v>207</v>
-      </c>
       <c r="R28" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="S28" s="16">
         <v>25</v>
       </c>
       <c r="T28" s="25" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
@@ -5023,13 +5023,13 @@
         <v>2</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F29" s="25">
         <v>5</v>
@@ -5049,28 +5049,28 @@
       <c r="K29" s="25"/>
       <c r="L29" s="25"/>
       <c r="M29" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="N29" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="N29" s="8" t="s">
+      <c r="O29" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="O29" s="31" t="s">
+      <c r="P29" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q29" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="P29" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q29" s="11" t="s">
-        <v>212</v>
-      </c>
       <c r="R29" s="16" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="S29" s="11">
         <v>26</v>
       </c>
       <c r="T29" s="25" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
@@ -5078,13 +5078,13 @@
         <v>2</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E30" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F30" s="37">
         <v>6</v>
@@ -5104,28 +5104,28 @@
       <c r="K30" s="37"/>
       <c r="L30" s="37"/>
       <c r="M30" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="N30" s="39" t="s">
         <v>214</v>
       </c>
-      <c r="N30" s="39" t="s">
+      <c r="O30" s="39" t="s">
         <v>215</v>
       </c>
-      <c r="O30" s="39" t="s">
+      <c r="P30" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q30" s="35" t="s">
         <v>216</v>
       </c>
-      <c r="P30" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q30" s="35" t="s">
-        <v>217</v>
-      </c>
       <c r="R30" s="35" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="S30" s="35">
         <v>27</v>
       </c>
       <c r="T30" s="37" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
@@ -5133,13 +5133,13 @@
         <v>2</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E31" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F31" s="37">
         <v>4</v>
@@ -5159,28 +5159,28 @@
       <c r="K31" s="37"/>
       <c r="L31" s="37"/>
       <c r="M31" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="N31" s="39" t="s">
         <v>279</v>
       </c>
-      <c r="N31" s="39" t="s">
+      <c r="O31" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="O31" s="39" t="s">
+      <c r="P31" s="36" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q31" s="35" t="s">
         <v>281</v>
       </c>
-      <c r="P31" s="36" t="s">
-        <v>489</v>
-      </c>
-      <c r="Q31" s="35" t="s">
+      <c r="R31" s="35" t="s">
         <v>282</v>
-      </c>
-      <c r="R31" s="35" t="s">
-        <v>283</v>
       </c>
       <c r="S31" s="35">
         <v>40</v>
       </c>
       <c r="T31" s="37" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
@@ -5188,13 +5188,13 @@
         <v>2</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E32" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F32" s="37">
         <v>9</v>
@@ -5214,28 +5214,28 @@
       <c r="K32" s="37"/>
       <c r="L32" s="37"/>
       <c r="M32" s="39" t="s">
+        <v>284</v>
+      </c>
+      <c r="N32" s="39" t="s">
         <v>285</v>
       </c>
-      <c r="N32" s="39" t="s">
+      <c r="O32" s="39" t="s">
         <v>286</v>
       </c>
-      <c r="O32" s="39" t="s">
+      <c r="P32" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q32" s="35" t="s">
         <v>287</v>
       </c>
-      <c r="P32" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q32" s="35" t="s">
+      <c r="R32" s="35" t="s">
         <v>288</v>
-      </c>
-      <c r="R32" s="35" t="s">
-        <v>289</v>
       </c>
       <c r="S32" s="35">
         <v>41</v>
       </c>
       <c r="T32" s="37" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
@@ -5243,13 +5243,13 @@
         <v>2</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E33" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F33" s="37">
         <v>10</v>
@@ -5269,28 +5269,28 @@
       <c r="K33" s="37"/>
       <c r="L33" s="37"/>
       <c r="M33" s="39" t="s">
+        <v>290</v>
+      </c>
+      <c r="N33" s="39" t="s">
         <v>291</v>
       </c>
-      <c r="N33" s="39" t="s">
+      <c r="O33" s="39" t="s">
         <v>292</v>
       </c>
-      <c r="O33" s="39" t="s">
+      <c r="P33" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q33" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="P33" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q33" s="35" t="s">
+      <c r="R33" s="35" t="s">
         <v>294</v>
-      </c>
-      <c r="R33" s="35" t="s">
-        <v>295</v>
       </c>
       <c r="S33" s="35">
         <v>42</v>
       </c>
       <c r="T33" s="37" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
@@ -5298,13 +5298,13 @@
         <v>2</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F34" s="37">
         <v>11</v>
@@ -5324,28 +5324,28 @@
       <c r="K34" s="37"/>
       <c r="L34" s="37"/>
       <c r="M34" s="39" t="s">
+        <v>296</v>
+      </c>
+      <c r="N34" s="40" t="s">
         <v>297</v>
       </c>
-      <c r="N34" s="40" t="s">
+      <c r="O34" s="39" t="s">
         <v>298</v>
       </c>
-      <c r="O34" s="39" t="s">
+      <c r="P34" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q34" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="P34" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q34" s="35" t="s">
+      <c r="R34" s="35" t="s">
         <v>300</v>
-      </c>
-      <c r="R34" s="35" t="s">
-        <v>301</v>
       </c>
       <c r="S34" s="35">
         <v>43</v>
       </c>
       <c r="T34" s="37" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
@@ -5353,13 +5353,13 @@
         <v>2</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F35" s="25">
         <v>0</v>
@@ -5379,28 +5379,28 @@
       <c r="K35" s="25"/>
       <c r="L35" s="25"/>
       <c r="M35" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="N35" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="O35" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="O35" s="8" t="s">
-        <v>299</v>
-      </c>
       <c r="P35" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q35" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="R35" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="S35" s="11">
         <v>44</v>
       </c>
       <c r="T35" s="25" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
@@ -5408,13 +5408,13 @@
         <v>2</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F36" s="25">
         <v>12</v>
@@ -5434,28 +5434,28 @@
       <c r="K36" s="25"/>
       <c r="L36" s="25"/>
       <c r="M36" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="N36" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="N36" s="8" t="s">
+      <c r="O36" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="O36" s="8" t="s">
-        <v>299</v>
-      </c>
       <c r="P36" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q36" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="R36" s="11" t="s">
         <v>304</v>
-      </c>
-      <c r="R36" s="11" t="s">
-        <v>305</v>
       </c>
       <c r="S36" s="16">
         <v>45</v>
       </c>
       <c r="T36" s="25" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
@@ -5463,13 +5463,13 @@
         <v>2</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F37" s="25">
         <v>1</v>
@@ -5489,28 +5489,28 @@
       <c r="K37" s="25"/>
       <c r="L37" s="25"/>
       <c r="M37" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="N37" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="N37" s="8" t="s">
+      <c r="O37" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="O37" s="8" t="s">
-        <v>299</v>
-      </c>
       <c r="P37" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q37" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="R37" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="S37" s="11">
         <v>46</v>
       </c>
       <c r="T37" s="25" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
@@ -5518,13 +5518,13 @@
         <v>2</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F38" s="25">
         <v>1</v>
@@ -5544,28 +5544,28 @@
       <c r="K38" s="25"/>
       <c r="L38" s="25"/>
       <c r="M38" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="N38" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="N38" s="8" t="s">
+      <c r="O38" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="O38" s="8" t="s">
-        <v>299</v>
-      </c>
       <c r="P38" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q38" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="R38" s="11" t="s">
         <v>308</v>
-      </c>
-      <c r="R38" s="11" t="s">
-        <v>309</v>
       </c>
       <c r="S38" s="16">
         <v>47</v>
       </c>
       <c r="T38" s="25" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
@@ -5573,13 +5573,13 @@
         <v>2</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F39" s="25">
         <v>2</v>
@@ -5599,28 +5599,28 @@
       <c r="K39" s="25"/>
       <c r="L39" s="25"/>
       <c r="M39" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="N39" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="N39" s="8" t="s">
+      <c r="O39" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="O39" s="31" t="s">
+      <c r="P39" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q39" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="P39" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q39" s="11" t="s">
+      <c r="R39" s="16" t="s">
         <v>314</v>
-      </c>
-      <c r="R39" s="16" t="s">
-        <v>315</v>
       </c>
       <c r="S39" s="11">
         <v>48</v>
       </c>
       <c r="T39" s="25" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
@@ -5628,13 +5628,13 @@
         <v>2</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E40" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F40" s="37">
         <v>3</v>
@@ -5654,28 +5654,28 @@
       <c r="K40" s="37"/>
       <c r="L40" s="37"/>
       <c r="M40" s="39" t="s">
+        <v>316</v>
+      </c>
+      <c r="N40" s="39" t="s">
         <v>317</v>
       </c>
-      <c r="N40" s="39" t="s">
+      <c r="O40" s="39" t="s">
         <v>318</v>
       </c>
-      <c r="O40" s="39" t="s">
+      <c r="P40" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q40" s="35" t="s">
         <v>319</v>
       </c>
-      <c r="P40" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q40" s="35" t="s">
+      <c r="R40" s="35" t="s">
         <v>320</v>
-      </c>
-      <c r="R40" s="35" t="s">
-        <v>321</v>
       </c>
       <c r="S40" s="35">
         <v>49</v>
       </c>
       <c r="T40" s="37" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
@@ -5683,13 +5683,13 @@
         <v>2</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E41" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F41" s="37">
         <v>13</v>
@@ -5709,28 +5709,28 @@
       <c r="K41" s="37"/>
       <c r="L41" s="37"/>
       <c r="M41" s="39" t="s">
+        <v>322</v>
+      </c>
+      <c r="N41" s="39" t="s">
         <v>323</v>
       </c>
-      <c r="N41" s="39" t="s">
+      <c r="O41" s="39" t="s">
         <v>324</v>
       </c>
-      <c r="O41" s="39" t="s">
+      <c r="P41" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q41" s="35" t="s">
         <v>325</v>
       </c>
-      <c r="P41" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q41" s="35" t="s">
+      <c r="R41" s="35" t="s">
         <v>326</v>
-      </c>
-      <c r="R41" s="35" t="s">
-        <v>327</v>
       </c>
       <c r="S41" s="35">
         <v>50</v>
       </c>
       <c r="T41" s="37" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
@@ -5738,13 +5738,13 @@
         <v>2</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E42" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F42" s="37">
         <v>14</v>
@@ -5764,28 +5764,28 @@
       <c r="K42" s="37"/>
       <c r="L42" s="37"/>
       <c r="M42" s="39" t="s">
+        <v>328</v>
+      </c>
+      <c r="N42" s="39" t="s">
         <v>329</v>
       </c>
-      <c r="N42" s="39" t="s">
+      <c r="O42" s="39" t="s">
         <v>330</v>
       </c>
-      <c r="O42" s="39" t="s">
+      <c r="P42" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q42" s="35" t="s">
         <v>331</v>
       </c>
-      <c r="P42" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q42" s="35" t="s">
-        <v>332</v>
-      </c>
       <c r="R42" s="35" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S42" s="35">
         <v>51</v>
       </c>
       <c r="T42" s="37" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
@@ -5793,13 +5793,13 @@
         <v>2</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E43" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F43" s="37">
         <v>4</v>
@@ -5819,28 +5819,28 @@
       <c r="K43" s="37"/>
       <c r="L43" s="37"/>
       <c r="M43" s="39" t="s">
+        <v>333</v>
+      </c>
+      <c r="N43" s="39" t="s">
         <v>334</v>
       </c>
-      <c r="N43" s="39" t="s">
+      <c r="O43" s="39" t="s">
         <v>335</v>
       </c>
-      <c r="O43" s="39" t="s">
+      <c r="P43" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" s="35" t="s">
         <v>336</v>
       </c>
-      <c r="P43" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q43" s="35" t="s">
+      <c r="R43" s="35" t="s">
         <v>337</v>
-      </c>
-      <c r="R43" s="35" t="s">
-        <v>338</v>
       </c>
       <c r="S43" s="35">
         <v>52</v>
       </c>
       <c r="T43" s="37" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
@@ -5848,13 +5848,13 @@
         <v>2</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D44" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="37" t="s">
         <v>13</v>
-      </c>
-      <c r="E44" s="37" t="s">
-        <v>14</v>
       </c>
       <c r="F44" s="37">
         <v>7</v>
@@ -5874,28 +5874,28 @@
       <c r="K44" s="37"/>
       <c r="L44" s="37"/>
       <c r="M44" s="39" t="s">
+        <v>243</v>
+      </c>
+      <c r="N44" s="40" t="s">
         <v>244</v>
       </c>
-      <c r="N44" s="40" t="s">
+      <c r="O44" s="39" t="s">
         <v>245</v>
       </c>
-      <c r="O44" s="39" t="s">
+      <c r="P44" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q44" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="P44" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q44" s="35" t="s">
-        <v>247</v>
-      </c>
       <c r="R44" s="35" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="S44" s="35">
         <v>33</v>
       </c>
       <c r="T44" s="37" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
@@ -5903,13 +5903,13 @@
         <v>2</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D45" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="25" t="s">
         <v>13</v>
-      </c>
-      <c r="E45" s="25" t="s">
-        <v>14</v>
       </c>
       <c r="F45" s="25">
         <v>9</v>
@@ -5929,28 +5929,28 @@
       <c r="K45" s="25"/>
       <c r="L45" s="25"/>
       <c r="M45" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="N45" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="N45" s="8" t="s">
+      <c r="O45" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="O45" s="8" t="s">
+      <c r="P45" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q45" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="P45" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q45" s="11" t="s">
-        <v>257</v>
-      </c>
       <c r="R45" s="11" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="S45" s="11">
         <v>35</v>
       </c>
       <c r="T45" s="25" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
@@ -5958,13 +5958,13 @@
         <v>2</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F46" s="25">
         <v>4</v>
@@ -5984,28 +5984,28 @@
       <c r="K46" s="25"/>
       <c r="L46" s="25"/>
       <c r="M46" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="N46" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="N46" s="8" t="s">
+      <c r="O46" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="O46" s="8" t="s">
+      <c r="P46" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q46" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="P46" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q46" s="11" t="s">
-        <v>262</v>
-      </c>
       <c r="R46" s="11" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="S46" s="16">
         <v>36</v>
       </c>
       <c r="T46" s="25" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
@@ -6013,13 +6013,13 @@
         <v>2</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D47" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="25" t="s">
         <v>13</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>14</v>
       </c>
       <c r="F47" s="25">
         <v>12</v>
@@ -6039,28 +6039,28 @@
       <c r="K47" s="25"/>
       <c r="L47" s="25"/>
       <c r="M47" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="N47" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="N47" s="8" t="s">
+      <c r="O47" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="O47" s="8" t="s">
+      <c r="P47" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q47" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="P47" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q47" s="11" t="s">
-        <v>267</v>
-      </c>
       <c r="R47" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="S47" s="11">
         <v>37</v>
       </c>
       <c r="T47" s="25" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
@@ -6068,13 +6068,13 @@
         <v>2</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D48" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="25" t="s">
         <v>13</v>
-      </c>
-      <c r="E48" s="25" t="s">
-        <v>14</v>
       </c>
       <c r="F48" s="25">
         <v>13</v>
@@ -6094,28 +6094,28 @@
       <c r="K48" s="25"/>
       <c r="L48" s="25"/>
       <c r="M48" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="N48" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="N48" s="8" t="s">
+      <c r="O48" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="O48" s="8" t="s">
+      <c r="P48" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q48" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="P48" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q48" s="11" t="s">
-        <v>272</v>
-      </c>
       <c r="R48" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="S48" s="16">
         <v>38</v>
       </c>
       <c r="T48" s="25" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
@@ -6123,13 +6123,13 @@
         <v>2</v>
       </c>
       <c r="C49" s="29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D49" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="25" t="s">
         <v>13</v>
-      </c>
-      <c r="E49" s="25" t="s">
-        <v>14</v>
       </c>
       <c r="F49" s="25">
         <v>14</v>
@@ -6149,28 +6149,28 @@
       <c r="K49" s="25"/>
       <c r="L49" s="25"/>
       <c r="M49" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="N49" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="N49" s="8" t="s">
+      <c r="O49" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="O49" s="31" t="s">
+      <c r="P49" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q49" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="P49" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q49" s="11" t="s">
-        <v>277</v>
-      </c>
       <c r="R49" s="16" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="S49" s="11">
         <v>39</v>
       </c>
       <c r="T49" s="25" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
@@ -6178,13 +6178,13 @@
         <v>2</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E50" s="37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F50" s="37">
         <v>5</v>
@@ -6202,32 +6202,32 @@
         <v>0</v>
       </c>
       <c r="K50" s="37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L50" s="37"/>
       <c r="M50" s="39" t="s">
+        <v>355</v>
+      </c>
+      <c r="N50" s="39" t="s">
         <v>356</v>
       </c>
-      <c r="N50" s="39" t="s">
+      <c r="O50" s="39" t="s">
         <v>357</v>
       </c>
-      <c r="O50" s="39" t="s">
+      <c r="P50" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q50" s="35" t="s">
         <v>358</v>
       </c>
-      <c r="P50" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q50" s="35" t="s">
+      <c r="R50" s="35" t="s">
         <v>359</v>
-      </c>
-      <c r="R50" s="35" t="s">
-        <v>360</v>
       </c>
       <c r="S50" s="35">
         <v>58</v>
       </c>
       <c r="T50" s="37" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
@@ -6235,13 +6235,13 @@
         <v>2</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D51" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="37" t="s">
         <v>13</v>
-      </c>
-      <c r="E51" s="37" t="s">
-        <v>14</v>
       </c>
       <c r="F51" s="37">
         <v>11</v>
@@ -6261,28 +6261,28 @@
       <c r="K51" s="37"/>
       <c r="L51" s="37"/>
       <c r="M51" s="39" t="s">
+        <v>398</v>
+      </c>
+      <c r="N51" s="39" t="s">
         <v>399</v>
       </c>
-      <c r="N51" s="39" t="s">
-        <v>400</v>
-      </c>
       <c r="O51" s="39" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="P51" s="36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q51" s="35" t="s">
+        <v>367</v>
+      </c>
+      <c r="R51" s="35" t="s">
         <v>368</v>
-      </c>
-      <c r="R51" s="35" t="s">
-        <v>369</v>
       </c>
       <c r="S51" s="35">
         <v>59</v>
       </c>
       <c r="T51" s="37" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.25">
@@ -6290,13 +6290,13 @@
         <v>2</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D52" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="37" t="s">
         <v>13</v>
-      </c>
-      <c r="E52" s="37" t="s">
-        <v>14</v>
       </c>
       <c r="F52" s="37">
         <v>13</v>
@@ -6314,32 +6314,32 @@
         <v>0</v>
       </c>
       <c r="K52" s="37" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L52" s="37"/>
       <c r="M52" s="39" t="s">
+        <v>505</v>
+      </c>
+      <c r="N52" s="39" t="s">
         <v>506</v>
       </c>
-      <c r="N52" s="39" t="s">
-        <v>507</v>
-      </c>
       <c r="O52" s="39" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="P52" s="36" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="Q52" s="35" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="R52" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="S52" s="35">
         <v>63</v>
       </c>
       <c r="T52" s="37" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.25">
@@ -6347,13 +6347,13 @@
         <v>2</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D53" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="37" t="s">
         <v>13</v>
-      </c>
-      <c r="E53" s="37" t="s">
-        <v>14</v>
       </c>
       <c r="F53" s="37">
         <v>16</v>
@@ -6371,32 +6371,32 @@
         <v>0</v>
       </c>
       <c r="K53" s="37" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="L53" s="37"/>
       <c r="M53" s="39" t="s">
+        <v>503</v>
+      </c>
+      <c r="N53" s="39" t="s">
         <v>504</v>
       </c>
-      <c r="N53" s="39" t="s">
-        <v>505</v>
-      </c>
       <c r="O53" s="39" t="s">
+        <v>426</v>
+      </c>
+      <c r="P53" s="36" t="s">
         <v>427</v>
       </c>
-      <c r="P53" s="36" t="s">
+      <c r="Q53" s="35" t="s">
         <v>428</v>
       </c>
-      <c r="Q53" s="35" t="s">
+      <c r="R53" s="35" t="s">
         <v>429</v>
-      </c>
-      <c r="R53" s="35" t="s">
-        <v>430</v>
       </c>
       <c r="S53" s="35">
         <v>66</v>
       </c>
       <c r="T53" s="37" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
@@ -6404,13 +6404,13 @@
         <v>2</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D54" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="37" t="s">
         <v>13</v>
-      </c>
-      <c r="E54" s="37" t="s">
-        <v>14</v>
       </c>
       <c r="F54" s="37">
         <v>20</v>
@@ -6428,32 +6428,32 @@
         <v>0</v>
       </c>
       <c r="K54" s="37" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L54" s="37"/>
       <c r="M54" s="39" t="s">
+        <v>465</v>
+      </c>
+      <c r="N54" s="40" t="s">
         <v>466</v>
       </c>
-      <c r="N54" s="40" t="s">
+      <c r="O54" s="39" t="s">
         <v>467</v>
       </c>
-      <c r="O54" s="39" t="s">
+      <c r="P54" s="36" t="s">
         <v>468</v>
       </c>
-      <c r="P54" s="36" t="s">
+      <c r="Q54" s="35" t="s">
         <v>469</v>
       </c>
-      <c r="Q54" s="35" t="s">
+      <c r="R54" s="35" t="s">
         <v>470</v>
-      </c>
-      <c r="R54" s="35" t="s">
-        <v>471</v>
       </c>
       <c r="S54" s="35">
         <v>71</v>
       </c>
       <c r="T54" s="37" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.25">
@@ -6461,13 +6461,13 @@
         <v>2</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D55" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="25" t="s">
         <v>13</v>
-      </c>
-      <c r="E55" s="25" t="s">
-        <v>14</v>
       </c>
       <c r="F55" s="25">
         <v>21</v>
@@ -6487,26 +6487,26 @@
       <c r="K55" s="25"/>
       <c r="L55" s="25"/>
       <c r="M55" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="N55" s="8" t="s">
         <v>473</v>
       </c>
-      <c r="N55" s="8" t="s">
-        <v>474</v>
-      </c>
       <c r="O55" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="P55" s="15"/>
       <c r="Q55" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="R55" s="11" t="s">
         <v>470</v>
-      </c>
-      <c r="R55" s="11" t="s">
-        <v>471</v>
       </c>
       <c r="S55" s="11">
         <v>71</v>
       </c>
       <c r="T55" s="25" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.25">
@@ -6514,13 +6514,13 @@
         <v>2</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F56" s="25">
         <v>1</v>
@@ -6540,28 +6540,28 @@
       <c r="K56" s="25"/>
       <c r="L56" s="25"/>
       <c r="M56" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N56" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="N56" s="8" t="s">
+      <c r="O56" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="O56" s="8" t="s">
+      <c r="P56" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q56" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="P56" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q56" s="11" t="s">
-        <v>143</v>
-      </c>
       <c r="R56" s="11" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="S56" s="16">
         <v>12</v>
       </c>
       <c r="T56" s="25" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.25">
@@ -6569,10 +6569,10 @@
         <v>2</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E57" s="25" t="s">
         <v>4</v>
@@ -6595,28 +6595,28 @@
       <c r="K57" s="25"/>
       <c r="L57" s="25"/>
       <c r="M57" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="N57" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="N57" s="8" t="s">
+      <c r="O57" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="O57" s="8" t="s">
+      <c r="P57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q57" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="P57" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q57" s="11" t="s">
-        <v>203</v>
-      </c>
       <c r="R57" s="16" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="S57" s="11">
         <v>24</v>
       </c>
       <c r="T57" s="25" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
@@ -6624,13 +6624,13 @@
         <v>2</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E58" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F58" s="25">
         <v>5</v>
@@ -6650,28 +6650,28 @@
       <c r="K58" s="25"/>
       <c r="L58" s="25"/>
       <c r="M58" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="N58" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="N58" s="8" t="s">
+      <c r="O58" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="O58" s="8" t="s">
+      <c r="P58" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q58" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="P58" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q58" s="11" t="s">
-        <v>222</v>
-      </c>
       <c r="R58" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="S58" s="16">
         <v>28</v>
       </c>
       <c r="T58" s="25" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.25">
@@ -6679,13 +6679,13 @@
         <v>2</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E59" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F59" s="25">
         <v>6</v>
@@ -6705,28 +6705,28 @@
       <c r="K59" s="25"/>
       <c r="L59" s="25"/>
       <c r="M59" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="N59" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="N59" s="8" t="s">
+      <c r="O59" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="O59" s="31" t="s">
+      <c r="P59" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q59" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="P59" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q59" s="11" t="s">
-        <v>227</v>
-      </c>
       <c r="R59" s="16" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="S59" s="11">
         <v>29</v>
       </c>
       <c r="T59" s="25" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.25">
@@ -6734,13 +6734,13 @@
         <v>2</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D60" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E60" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F60" s="37">
         <v>7</v>
@@ -6759,31 +6759,31 @@
       </c>
       <c r="K60" s="37"/>
       <c r="L60" s="37" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M60" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="N60" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="N60" s="39" t="s">
+      <c r="O60" s="39" t="s">
         <v>230</v>
       </c>
-      <c r="O60" s="39" t="s">
+      <c r="P60" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q60" s="35" t="s">
         <v>231</v>
       </c>
-      <c r="P60" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q60" s="35" t="s">
-        <v>232</v>
-      </c>
       <c r="R60" s="35" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="S60" s="35">
         <v>30</v>
       </c>
       <c r="T60" s="37" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.25">
@@ -6791,13 +6791,13 @@
         <v>2</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D61" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E61" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F61" s="37">
         <v>7</v>
@@ -6816,31 +6816,31 @@
       </c>
       <c r="K61" s="37"/>
       <c r="L61" s="37" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M61" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="N61" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="N61" s="39" t="s">
+      <c r="O61" s="39" t="s">
         <v>235</v>
       </c>
-      <c r="O61" s="39" t="s">
+      <c r="P61" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q61" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="P61" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q61" s="35" t="s">
-        <v>237</v>
-      </c>
       <c r="R61" s="35" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="S61" s="35">
         <v>31</v>
       </c>
       <c r="T61" s="37" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.25">
@@ -6848,13 +6848,13 @@
         <v>2</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E62" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F62" s="37">
         <v>2</v>
@@ -6874,28 +6874,28 @@
       <c r="K62" s="37"/>
       <c r="L62" s="37"/>
       <c r="M62" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="N62" s="39" t="s">
         <v>239</v>
       </c>
-      <c r="N62" s="39" t="s">
+      <c r="O62" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="O62" s="39" t="s">
+      <c r="P62" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q62" s="35" t="s">
         <v>241</v>
       </c>
-      <c r="P62" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q62" s="35" t="s">
-        <v>242</v>
-      </c>
       <c r="R62" s="35" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="S62" s="35">
         <v>32</v>
       </c>
       <c r="T62" s="37" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.25">
@@ -6903,13 +6903,13 @@
         <v>2</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E63" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F63" s="37">
         <v>8</v>
@@ -6929,28 +6929,28 @@
       <c r="K63" s="37"/>
       <c r="L63" s="37"/>
       <c r="M63" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="N63" s="39" t="s">
         <v>249</v>
       </c>
-      <c r="N63" s="39" t="s">
+      <c r="O63" s="39" t="s">
         <v>250</v>
       </c>
-      <c r="O63" s="39" t="s">
+      <c r="P63" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q63" s="35" t="s">
         <v>251</v>
       </c>
-      <c r="P63" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q63" s="35" t="s">
-        <v>252</v>
-      </c>
       <c r="R63" s="35" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="S63" s="35">
         <v>34</v>
       </c>
       <c r="T63" s="37" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.25">
@@ -6958,13 +6958,13 @@
         <v>2</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E64" s="37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F64" s="37">
         <v>4</v>
@@ -6984,28 +6984,28 @@
       <c r="K64" s="37"/>
       <c r="L64" s="37"/>
       <c r="M64" s="39" t="s">
+        <v>296</v>
+      </c>
+      <c r="N64" s="40" t="s">
         <v>297</v>
       </c>
-      <c r="N64" s="40" t="s">
+      <c r="O64" s="39" t="s">
         <v>298</v>
       </c>
-      <c r="O64" s="39" t="s">
-        <v>299</v>
-      </c>
       <c r="P64" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q64" s="35" t="s">
+        <v>339</v>
+      </c>
+      <c r="R64" s="35" t="s">
         <v>340</v>
-      </c>
-      <c r="R64" s="35" t="s">
-        <v>341</v>
       </c>
       <c r="S64" s="35">
         <v>53</v>
       </c>
       <c r="T64" s="37" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="65" spans="2:20" x14ac:dyDescent="0.25">
@@ -7013,13 +7013,13 @@
         <v>2</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E65" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F65" s="25">
         <v>3</v>
@@ -7039,28 +7039,28 @@
       <c r="K65" s="25"/>
       <c r="L65" s="25"/>
       <c r="M65" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="N65" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="N65" s="8" t="s">
+      <c r="O65" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="O65" s="8" t="s">
-        <v>299</v>
-      </c>
       <c r="P65" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q65" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="R65" s="11" t="s">
         <v>343</v>
-      </c>
-      <c r="R65" s="11" t="s">
-        <v>344</v>
       </c>
       <c r="S65" s="11">
         <v>54</v>
       </c>
       <c r="T65" s="25" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="66" spans="2:20" x14ac:dyDescent="0.25">
@@ -7068,13 +7068,13 @@
         <v>2</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D66" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E66" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F66" s="25">
         <v>4</v>
@@ -7094,28 +7094,28 @@
       <c r="K66" s="25"/>
       <c r="L66" s="25"/>
       <c r="M66" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="N66" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="N66" s="8" t="s">
-        <v>446</v>
-      </c>
       <c r="O66" s="8" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="P66" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q66" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="R66" s="11" t="s">
         <v>346</v>
-      </c>
-      <c r="R66" s="11" t="s">
-        <v>347</v>
       </c>
       <c r="S66" s="16">
         <v>55</v>
       </c>
       <c r="T66" s="25" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="67" spans="2:20" x14ac:dyDescent="0.25">
@@ -7123,13 +7123,13 @@
         <v>2</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D67" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E67" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F67" s="25">
         <v>5</v>
@@ -7149,28 +7149,28 @@
       <c r="K67" s="25"/>
       <c r="L67" s="25"/>
       <c r="M67" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="N67" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="N67" s="8" t="s">
+      <c r="O67" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="O67" s="8" t="s">
-        <v>443</v>
-      </c>
       <c r="P67" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q67" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="R67" s="16" t="s">
         <v>349</v>
-      </c>
-      <c r="R67" s="16" t="s">
-        <v>350</v>
       </c>
       <c r="S67" s="11">
         <v>56</v>
       </c>
       <c r="T67" s="25" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="68" spans="2:20" x14ac:dyDescent="0.25">
@@ -7178,13 +7178,13 @@
         <v>2</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D68" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E68" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F68" s="25">
         <v>6</v>
@@ -7204,28 +7204,28 @@
       <c r="K68" s="25"/>
       <c r="L68" s="25"/>
       <c r="M68" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="N68" s="8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="O68" s="8" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="P68" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q68" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="R68" s="11" t="s">
         <v>352</v>
-      </c>
-      <c r="R68" s="11" t="s">
-        <v>353</v>
       </c>
       <c r="S68" s="16">
         <v>57</v>
       </c>
       <c r="T68" s="25" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="69" spans="2:20" x14ac:dyDescent="0.25">
@@ -7233,13 +7233,13 @@
         <v>2</v>
       </c>
       <c r="C69" s="29" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E69" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F69" s="25">
         <v>5</v>
@@ -7257,32 +7257,32 @@
         <v>0</v>
       </c>
       <c r="K69" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L69" s="25"/>
       <c r="M69" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="N69" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="N69" s="8" t="s">
+      <c r="O69" s="31" t="s">
         <v>363</v>
       </c>
-      <c r="O69" s="31" t="s">
+      <c r="P69" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q69" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="P69" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q69" s="11" t="s">
+      <c r="R69" s="16" t="s">
         <v>365</v>
-      </c>
-      <c r="R69" s="16" t="s">
-        <v>366</v>
       </c>
       <c r="S69" s="11">
         <v>60</v>
       </c>
       <c r="T69" s="25" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="70" spans="2:20" x14ac:dyDescent="0.25">
@@ -7290,13 +7290,13 @@
         <v>2</v>
       </c>
       <c r="C70" s="32" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D70" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E70" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F70" s="37">
         <v>6</v>
@@ -7314,32 +7314,32 @@
         <v>0</v>
       </c>
       <c r="K70" s="37" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L70" s="37"/>
       <c r="M70" s="39" t="s">
+        <v>501</v>
+      </c>
+      <c r="N70" s="39" t="s">
         <v>502</v>
       </c>
-      <c r="N70" s="39" t="s">
-        <v>503</v>
-      </c>
       <c r="O70" s="39" t="s">
+        <v>412</v>
+      </c>
+      <c r="P70" s="36" t="s">
         <v>413</v>
       </c>
-      <c r="P70" s="36" t="s">
-        <v>414</v>
-      </c>
       <c r="Q70" s="35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="R70" s="35" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="S70" s="35">
         <v>61</v>
       </c>
       <c r="T70" s="37" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="71" spans="2:20" x14ac:dyDescent="0.25">
@@ -7347,13 +7347,13 @@
         <v>2</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D71" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E71" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F71" s="37">
         <v>12</v>
@@ -7371,30 +7371,30 @@
         <v>1</v>
       </c>
       <c r="K71" s="37" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L71" s="37"/>
       <c r="M71" s="39" t="s">
+        <v>499</v>
+      </c>
+      <c r="N71" s="39" t="s">
         <v>500</v>
       </c>
-      <c r="N71" s="39" t="s">
-        <v>501</v>
-      </c>
       <c r="O71" s="39" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="P71" s="36"/>
       <c r="Q71" s="35" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="R71" s="35" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="S71" s="35">
         <v>62</v>
       </c>
       <c r="T71" s="37" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="72" spans="2:20" x14ac:dyDescent="0.25">
@@ -7402,13 +7402,13 @@
         <v>2</v>
       </c>
       <c r="C72" s="32" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D72" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E72" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F72" s="37">
         <v>14</v>
@@ -7426,32 +7426,32 @@
         <v>0</v>
       </c>
       <c r="K72" s="37" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="L72" s="37"/>
       <c r="M72" s="39" t="s">
+        <v>491</v>
+      </c>
+      <c r="N72" s="39" t="s">
         <v>492</v>
       </c>
-      <c r="N72" s="39" t="s">
+      <c r="O72" s="39" t="s">
         <v>493</v>
       </c>
-      <c r="O72" s="39" t="s">
-        <v>494</v>
-      </c>
       <c r="P72" s="36" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q72" s="35" t="s">
         <v>417</v>
       </c>
-      <c r="Q72" s="35" t="s">
+      <c r="R72" s="35" t="s">
         <v>418</v>
-      </c>
-      <c r="R72" s="35" t="s">
-        <v>419</v>
       </c>
       <c r="S72" s="35">
         <v>64</v>
       </c>
       <c r="T72" s="37" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="73" spans="2:20" x14ac:dyDescent="0.25">
@@ -7459,13 +7459,13 @@
         <v>2</v>
       </c>
       <c r="C73" s="32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D73" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E73" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F73" s="37">
         <v>15</v>
@@ -7483,32 +7483,32 @@
         <v>0</v>
       </c>
       <c r="K73" s="37" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="L73" s="37"/>
       <c r="M73" s="39" t="s">
+        <v>489</v>
+      </c>
+      <c r="N73" s="39" t="s">
         <v>490</v>
       </c>
-      <c r="N73" s="39" t="s">
-        <v>491</v>
-      </c>
       <c r="O73" s="39" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="P73" s="36" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q73" s="35" t="s">
         <v>422</v>
       </c>
-      <c r="Q73" s="35" t="s">
+      <c r="R73" s="35" t="s">
         <v>423</v>
-      </c>
-      <c r="R73" s="35" t="s">
-        <v>424</v>
       </c>
       <c r="S73" s="35">
         <v>65</v>
       </c>
       <c r="T73" s="37" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="74" spans="2:20" x14ac:dyDescent="0.25">
@@ -7516,13 +7516,13 @@
         <v>2</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D74" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E74" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F74" s="37">
         <v>17</v>
@@ -7541,31 +7541,31 @@
       </c>
       <c r="K74" s="37"/>
       <c r="L74" s="37" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M74" s="39" t="s">
+        <v>497</v>
+      </c>
+      <c r="N74" s="40" t="s">
         <v>498</v>
       </c>
-      <c r="N74" s="40" t="s">
-        <v>499</v>
-      </c>
       <c r="O74" s="39" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P74" s="36" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q74" s="35" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="R74" s="35" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="S74" s="35">
         <v>67</v>
       </c>
       <c r="T74" s="37" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="75" spans="2:20" x14ac:dyDescent="0.25">
@@ -7573,13 +7573,13 @@
         <v>2</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E75" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F75" s="25">
         <v>7</v>
@@ -7598,31 +7598,31 @@
       </c>
       <c r="K75" s="25"/>
       <c r="L75" s="25" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="M75" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="N75" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="N75" s="8" t="s">
-        <v>497</v>
-      </c>
       <c r="O75" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="P75" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q75" s="11" t="s">
         <v>434</v>
       </c>
-      <c r="P75" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q75" s="11" t="s">
-        <v>435</v>
-      </c>
       <c r="R75" s="11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="S75" s="11">
         <v>68</v>
       </c>
       <c r="T75" s="25" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="76" spans="2:20" x14ac:dyDescent="0.25">
@@ -7630,13 +7630,13 @@
         <v>2</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E76" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F76" s="25">
         <v>18</v>
@@ -7654,32 +7654,32 @@
         <v>0</v>
       </c>
       <c r="K76" s="25" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L76" s="25"/>
       <c r="M76" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="N76" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="N76" s="8" t="s">
+      <c r="O76" s="8" t="s">
         <v>453</v>
       </c>
-      <c r="O76" s="8" t="s">
+      <c r="P76" s="15" t="s">
         <v>454</v>
       </c>
-      <c r="P76" s="15" t="s">
+      <c r="Q76" s="11" t="s">
         <v>455</v>
       </c>
-      <c r="Q76" s="11" t="s">
+      <c r="R76" s="11" t="s">
         <v>456</v>
-      </c>
-      <c r="R76" s="11" t="s">
-        <v>457</v>
       </c>
       <c r="S76" s="16">
         <v>69</v>
       </c>
       <c r="T76" s="25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="77" spans="2:20" x14ac:dyDescent="0.25">
@@ -7687,13 +7687,13 @@
         <v>2</v>
       </c>
       <c r="C77" s="29" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D77" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E77" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F77" s="25">
         <v>19</v>
@@ -7711,32 +7711,32 @@
         <v>0</v>
       </c>
       <c r="K77" s="25" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L77" s="25"/>
       <c r="M77" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="N77" s="8" t="s">
         <v>459</v>
       </c>
-      <c r="N77" s="8" t="s">
+      <c r="O77" s="8" t="s">
         <v>460</v>
       </c>
-      <c r="O77" s="8" t="s">
+      <c r="P77" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="P77" s="15" t="s">
+      <c r="Q77" s="11" t="s">
         <v>462</v>
       </c>
-      <c r="Q77" s="11" t="s">
+      <c r="R77" s="16" t="s">
         <v>463</v>
-      </c>
-      <c r="R77" s="16" t="s">
-        <v>464</v>
       </c>
       <c r="S77" s="11">
         <v>70</v>
       </c>
       <c r="T77" s="25" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="78" spans="2:20" x14ac:dyDescent="0.25">
@@ -7744,13 +7744,13 @@
         <v>2</v>
       </c>
       <c r="C78" s="29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D78" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" s="25" t="s">
         <v>13</v>
-      </c>
-      <c r="E78" s="25" t="s">
-        <v>14</v>
       </c>
       <c r="F78" s="25">
         <v>20</v>
@@ -7768,32 +7768,32 @@
         <v>0</v>
       </c>
       <c r="K78" s="25" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L78" s="25"/>
       <c r="M78" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="N78" s="8" t="s">
         <v>478</v>
       </c>
-      <c r="N78" s="8" t="s">
+      <c r="O78" s="8" t="s">
         <v>479</v>
       </c>
-      <c r="O78" s="8" t="s">
+      <c r="P78" s="15" t="s">
         <v>480</v>
       </c>
-      <c r="P78" s="15" t="s">
+      <c r="Q78" s="11" t="s">
         <v>481</v>
       </c>
-      <c r="Q78" s="11" t="s">
-        <v>482</v>
-      </c>
       <c r="R78" s="11" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="S78" s="16">
         <v>73</v>
       </c>
       <c r="T78" s="25" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="79" spans="2:20" x14ac:dyDescent="0.25">
@@ -7801,13 +7801,13 @@
         <v>2</v>
       </c>
       <c r="C79" s="29" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D79" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="25" t="s">
         <v>13</v>
-      </c>
-      <c r="E79" s="25" t="s">
-        <v>14</v>
       </c>
       <c r="F79" s="25">
         <v>21</v>
@@ -7825,32 +7825,32 @@
         <v>0</v>
       </c>
       <c r="K79" s="25" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L79" s="25"/>
       <c r="M79" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="N79" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="N79" s="8" t="s">
+      <c r="O79" s="31" t="s">
         <v>485</v>
       </c>
-      <c r="O79" s="31" t="s">
+      <c r="P79" s="15" t="s">
         <v>486</v>
       </c>
-      <c r="P79" s="15" t="s">
+      <c r="Q79" s="11" t="s">
         <v>487</v>
       </c>
-      <c r="Q79" s="11" t="s">
-        <v>488</v>
-      </c>
       <c r="R79" s="16" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="S79" s="11">
         <v>74</v>
       </c>
       <c r="T79" s="25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="80" spans="2:20" x14ac:dyDescent="0.25">
@@ -7858,13 +7858,13 @@
         <v>2</v>
       </c>
       <c r="C80" s="29" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D80" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="25" t="s">
         <v>13</v>
-      </c>
-      <c r="E80" s="25" t="s">
-        <v>14</v>
       </c>
       <c r="F80" s="25">
         <v>22</v>
@@ -7882,38 +7882,38 @@
         <v>0</v>
       </c>
       <c r="K80" s="25" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L80" s="25"/>
       <c r="M80" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="N80" s="8" t="s">
         <v>625</v>
       </c>
-      <c r="N80" s="8" t="s">
+      <c r="O80" s="31" t="s">
         <v>626</v>
       </c>
-      <c r="O80" s="31" t="s">
+      <c r="P80" s="15" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q80" s="11" t="s">
         <v>627</v>
       </c>
-      <c r="P80" s="15" t="s">
-        <v>630</v>
-      </c>
-      <c r="Q80" s="11" t="s">
+      <c r="R80" s="16" t="s">
         <v>628</v>
-      </c>
-      <c r="R80" s="16" t="s">
-        <v>629</v>
       </c>
       <c r="S80" s="11">
         <v>75</v>
       </c>
       <c r="T80" s="25" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="81" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="82" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B82" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -7933,45 +7933,45 @@
     </row>
     <row r="84" spans="2:17" ht="135" x14ac:dyDescent="0.25">
       <c r="B84" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="C84" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="21" t="s">
         <v>371</v>
       </c>
-      <c r="C84" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D84" s="21" t="s">
+      <c r="E84" s="21" t="s">
         <v>372</v>
       </c>
-      <c r="E84" s="21" t="s">
+      <c r="F84" s="21" t="s">
         <v>373</v>
       </c>
-      <c r="F84" s="21" t="s">
+      <c r="G84" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="G84" s="21" t="s">
+      <c r="H84" s="21" t="s">
         <v>375</v>
       </c>
-      <c r="H84" s="21" t="s">
+      <c r="I84" s="22" t="s">
         <v>376</v>
       </c>
-      <c r="I84" s="22" t="s">
+      <c r="J84" s="22" t="s">
         <v>377</v>
-      </c>
-      <c r="J84" s="22" t="s">
-        <v>378</v>
       </c>
       <c r="K84" s="22"/>
       <c r="L84" s="22"/>
       <c r="M84" s="22" t="s">
+        <v>378</v>
+      </c>
+      <c r="N84" s="22" t="s">
         <v>379</v>
       </c>
-      <c r="N84" s="22" t="s">
+      <c r="O84" s="22" t="s">
         <v>380</v>
       </c>
-      <c r="O84" s="22" t="s">
+      <c r="P84" s="22" t="s">
         <v>381</v>
-      </c>
-      <c r="P84" s="22" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="85" spans="2:17" x14ac:dyDescent="0.25">
@@ -7979,7 +7979,7 @@
         <v>2</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D85" s="25">
         <v>1.3</v>
@@ -8018,7 +8018,7 @@
         <v>2</v>
       </c>
       <c r="C86" s="24" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D86" s="25">
         <v>1.3</v>
@@ -8039,7 +8039,7 @@
         <v>0.5</v>
       </c>
       <c r="J86" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K86" s="8"/>
       <c r="L86" s="8"/>
@@ -8059,7 +8059,7 @@
         <v>2</v>
       </c>
       <c r="C87" s="27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D87" s="25">
         <v>1.3</v>
@@ -8080,7 +8080,7 @@
         <v>0.5</v>
       </c>
       <c r="J87" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K87" s="8"/>
       <c r="L87" s="8"/>
@@ -8100,7 +8100,7 @@
         <v>2</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D88" s="25">
         <v>1.3</v>
@@ -8124,7 +8124,7 @@
       <c r="K88" s="8"/>
       <c r="L88" s="8"/>
       <c r="M88" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="N88" s="8" t="b">
         <v>0</v>
@@ -8141,7 +8141,7 @@
         <v>2</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D89" s="25">
         <v>1.3</v>
@@ -8176,7 +8176,7 @@
         <v>2</v>
       </c>
       <c r="C90" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D90" s="25">
         <v>1.3</v>
@@ -8197,7 +8197,7 @@
         <v>0.5</v>
       </c>
       <c r="J90" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K90" s="8"/>
       <c r="L90" s="8"/>
@@ -8215,7 +8215,7 @@
     <row r="91" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="92" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B92" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -8236,19 +8236,19 @@
     </row>
     <row r="94" spans="2:17" ht="123" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="2:17" x14ac:dyDescent="0.25">
@@ -8256,16 +8256,16 @@
         <v>2</v>
       </c>
       <c r="C95" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D95" s="13">
+        <v>0</v>
+      </c>
+      <c r="E95" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D95" s="13">
-        <v>0</v>
-      </c>
-      <c r="E95" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="F95" s="28" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="96" spans="2:17" x14ac:dyDescent="0.25">
@@ -8273,16 +8273,16 @@
         <v>2</v>
       </c>
       <c r="C96" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D96" s="18">
         <v>1</v>
       </c>
       <c r="E96" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F96" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
@@ -8290,16 +8290,16 @@
         <v>2</v>
       </c>
       <c r="C97" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D97" s="13">
         <v>2</v>
       </c>
       <c r="E97" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F97" s="28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
@@ -8316,7 +8316,7 @@
         <v>5</v>
       </c>
       <c r="F98" s="28" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
@@ -8324,16 +8324,16 @@
         <v>2</v>
       </c>
       <c r="C99" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D99" s="13">
         <v>4</v>
       </c>
       <c r="E99" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F99" s="28" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
@@ -8341,16 +8341,16 @@
         <v>2</v>
       </c>
       <c r="C100" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D100" s="13">
         <v>5</v>
       </c>
       <c r="E100" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F100" s="28" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
@@ -8358,16 +8358,16 @@
         <v>2</v>
       </c>
       <c r="C101" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D101" s="13">
         <v>6</v>
       </c>
       <c r="E101" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F101" s="28" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renatus pet should be hidden, as is not implemented
Former-commit-id: 71f618306874b7d71ee315d8e26eb40d25074d40
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Pets.xlsx
+++ b/Docs/Content/HungryDragonContent_Pets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2503,13 +2503,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -2519,6 +2512,13 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -3196,13 +3196,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3232,6 +3225,13 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3281,7 +3281,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="petDefinitions2" displayName="petDefinitions2" ref="B4:T80" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" headerRowBorderDxfId="27" tableBorderDxfId="28" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="petDefinitions2" displayName="petDefinitions2" ref="B4:T80" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B4:T80"/>
   <sortState ref="B5:T77">
     <sortCondition ref="D4:D77"/>
@@ -3316,7 +3316,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B94:F101" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B94:F101" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B94:F101"/>
   <sortState ref="B95:F101">
     <sortCondition ref="D77:D84"/>
@@ -3600,8 +3600,8 @@
   </sheetPr>
   <dimension ref="B1:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="H34" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7040,7 +7040,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J65" s="25" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
xml was ok (petCategories) but not excel. Also minor fix in english until localization
Former-commit-id: 27819ac2378bcf866c586f6b3b76ad83306bf598
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Pets.xlsx
+++ b/Docs/Content/HungryDragonContent_Pets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="638">
   <si>
     <t>[sku]</t>
   </si>
@@ -1951,12 +1951,21 @@
   <si>
     <t>trash_eater_better</t>
   </si>
+  <si>
+    <t>baby</t>
+  </si>
+  <si>
+    <t>icon_baby</t>
+  </si>
+  <si>
+    <t>TID_PET_CATEGORY_BABY</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1996,6 +2005,17 @@
       <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2238,7 +2258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2360,6 +2380,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3316,8 +3345,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B94:F101" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B94:F101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B94:F102" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B94:F102"/>
   <sortState ref="B95:F101">
     <sortCondition ref="D77:D84"/>
   </sortState>
@@ -3598,13 +3627,13 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:T101"/>
+  <dimension ref="B1:T102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H34" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
@@ -3626,8 +3655,8 @@
     <col min="20" max="20" width="41.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:20" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:20" ht="23.25">
       <c r="B2" s="1" t="s">
         <v>63</v>
       </c>
@@ -3644,11 +3673,11 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:20" ht="104.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:20" ht="104.25">
       <c r="B4" s="3" t="s">
         <v>64</v>
       </c>
@@ -3707,7 +3736,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20">
       <c r="B5" s="33" t="s">
         <v>2</v>
       </c>
@@ -3762,7 +3791,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20">
       <c r="B6" s="33" t="s">
         <v>2</v>
       </c>
@@ -3817,7 +3846,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20">
       <c r="B7" s="34" t="s">
         <v>2</v>
       </c>
@@ -3872,7 +3901,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20">
       <c r="B8" s="34" t="s">
         <v>2</v>
       </c>
@@ -3927,7 +3956,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20">
       <c r="B9" s="34" t="s">
         <v>2</v>
       </c>
@@ -3982,7 +4011,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20">
       <c r="B10" s="41" t="s">
         <v>2</v>
       </c>
@@ -4037,7 +4066,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20">
       <c r="B11" s="41" t="s">
         <v>2</v>
       </c>
@@ -4092,7 +4121,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20">
       <c r="B12" s="41" t="s">
         <v>2</v>
       </c>
@@ -4147,7 +4176,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20">
       <c r="B13" s="41" t="s">
         <v>2</v>
       </c>
@@ -4202,7 +4231,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20">
       <c r="B14" s="41" t="s">
         <v>2</v>
       </c>
@@ -4257,7 +4286,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20">
       <c r="B15" s="33" t="s">
         <v>2</v>
       </c>
@@ -4312,7 +4341,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20">
       <c r="B16" s="33" t="s">
         <v>2</v>
       </c>
@@ -4367,7 +4396,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20">
       <c r="B17" s="34" t="s">
         <v>2</v>
       </c>
@@ -4422,7 +4451,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20">
       <c r="B18" s="34" t="s">
         <v>2</v>
       </c>
@@ -4477,7 +4506,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20">
       <c r="B19" s="34" t="s">
         <v>2</v>
       </c>
@@ -4532,7 +4561,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20">
       <c r="B20" s="41" t="s">
         <v>2</v>
       </c>
@@ -4587,7 +4616,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20">
       <c r="B21" s="41" t="s">
         <v>2</v>
       </c>
@@ -4642,7 +4671,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20">
       <c r="B22" s="41" t="s">
         <v>2</v>
       </c>
@@ -4697,7 +4726,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20">
       <c r="B23" s="41" t="s">
         <v>2</v>
       </c>
@@ -4752,7 +4781,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20">
       <c r="B24" s="41" t="s">
         <v>2</v>
       </c>
@@ -4807,7 +4836,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20">
       <c r="B25" s="33" t="s">
         <v>2</v>
       </c>
@@ -4862,7 +4891,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20">
       <c r="B26" s="33" t="s">
         <v>2</v>
       </c>
@@ -4917,7 +4946,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20">
       <c r="B27" s="34" t="s">
         <v>2</v>
       </c>
@@ -4972,7 +5001,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20">
       <c r="B28" s="34" t="s">
         <v>2</v>
       </c>
@@ -5027,7 +5056,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20">
       <c r="B29" s="34" t="s">
         <v>2</v>
       </c>
@@ -5082,7 +5111,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20">
       <c r="B30" s="41" t="s">
         <v>2</v>
       </c>
@@ -5137,7 +5166,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20">
       <c r="B31" s="41" t="s">
         <v>2</v>
       </c>
@@ -5192,7 +5221,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20">
       <c r="B32" s="41" t="s">
         <v>2</v>
       </c>
@@ -5247,7 +5276,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20">
       <c r="B33" s="41" t="s">
         <v>2</v>
       </c>
@@ -5302,7 +5331,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:20">
       <c r="B34" s="41" t="s">
         <v>2</v>
       </c>
@@ -5357,7 +5386,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20">
       <c r="B35" s="33" t="s">
         <v>2</v>
       </c>
@@ -5412,7 +5441,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20">
       <c r="B36" s="33" t="s">
         <v>2</v>
       </c>
@@ -5467,7 +5496,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:20">
       <c r="B37" s="34" t="s">
         <v>2</v>
       </c>
@@ -5522,7 +5551,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:20">
       <c r="B38" s="34" t="s">
         <v>2</v>
       </c>
@@ -5577,7 +5606,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:20">
       <c r="B39" s="34" t="s">
         <v>2</v>
       </c>
@@ -5632,7 +5661,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:20">
       <c r="B40" s="41" t="s">
         <v>2</v>
       </c>
@@ -5687,7 +5716,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20">
       <c r="B41" s="41" t="s">
         <v>2</v>
       </c>
@@ -5742,7 +5771,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:20">
       <c r="B42" s="41" t="s">
         <v>2</v>
       </c>
@@ -5797,7 +5826,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:20">
       <c r="B43" s="41" t="s">
         <v>2</v>
       </c>
@@ -5852,7 +5881,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20">
       <c r="B44" s="41" t="s">
         <v>2</v>
       </c>
@@ -5907,7 +5936,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:20">
       <c r="B45" s="33" t="s">
         <v>2</v>
       </c>
@@ -5962,7 +5991,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:20">
       <c r="B46" s="33" t="s">
         <v>2</v>
       </c>
@@ -6017,7 +6046,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:20">
       <c r="B47" s="34" t="s">
         <v>2</v>
       </c>
@@ -6072,7 +6101,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:20">
       <c r="B48" s="34" t="s">
         <v>2</v>
       </c>
@@ -6127,7 +6156,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:20">
       <c r="B49" s="34" t="s">
         <v>2</v>
       </c>
@@ -6182,7 +6211,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:20">
       <c r="B50" s="41" t="s">
         <v>2</v>
       </c>
@@ -6239,7 +6268,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:20">
       <c r="B51" s="41" t="s">
         <v>2</v>
       </c>
@@ -6294,7 +6323,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:20">
       <c r="B52" s="41" t="s">
         <v>2</v>
       </c>
@@ -6351,7 +6380,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:20">
       <c r="B53" s="41" t="s">
         <v>2</v>
       </c>
@@ -6408,7 +6437,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:20">
       <c r="B54" s="41" t="s">
         <v>2</v>
       </c>
@@ -6465,7 +6494,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:20">
       <c r="B55" s="33" t="s">
         <v>2</v>
       </c>
@@ -6518,7 +6547,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:20">
       <c r="B56" s="33" t="s">
         <v>2</v>
       </c>
@@ -6573,7 +6602,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:20">
       <c r="B57" s="34" t="s">
         <v>2</v>
       </c>
@@ -6628,7 +6657,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:20">
       <c r="B58" s="34" t="s">
         <v>2</v>
       </c>
@@ -6683,7 +6712,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="59" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:20">
       <c r="B59" s="34" t="s">
         <v>2</v>
       </c>
@@ -6738,7 +6767,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="60" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:20">
       <c r="B60" s="41" t="s">
         <v>2</v>
       </c>
@@ -6795,7 +6824,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="61" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:20">
       <c r="B61" s="41" t="s">
         <v>2</v>
       </c>
@@ -6852,7 +6881,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:20">
       <c r="B62" s="41" t="s">
         <v>2</v>
       </c>
@@ -6907,7 +6936,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="63" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:20">
       <c r="B63" s="41" t="s">
         <v>2</v>
       </c>
@@ -6962,7 +6991,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="64" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:20">
       <c r="B64" s="41" t="s">
         <v>2</v>
       </c>
@@ -7017,7 +7046,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="65" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:20">
       <c r="B65" s="33" t="s">
         <v>2</v>
       </c>
@@ -7072,7 +7101,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="66" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:20">
       <c r="B66" s="33" t="s">
         <v>2</v>
       </c>
@@ -7127,7 +7156,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="67" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:20">
       <c r="B67" s="34" t="s">
         <v>2</v>
       </c>
@@ -7182,7 +7211,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="68" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:20">
       <c r="B68" s="34" t="s">
         <v>2</v>
       </c>
@@ -7237,7 +7266,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="69" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:20">
       <c r="B69" s="34" t="s">
         <v>2</v>
       </c>
@@ -7294,7 +7323,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="70" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:20">
       <c r="B70" s="41" t="s">
         <v>2</v>
       </c>
@@ -7351,7 +7380,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="71" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:20">
       <c r="B71" s="41" t="s">
         <v>2</v>
       </c>
@@ -7406,7 +7435,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="72" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:20">
       <c r="B72" s="41" t="s">
         <v>2</v>
       </c>
@@ -7463,7 +7492,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="73" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:20">
       <c r="B73" s="41" t="s">
         <v>2</v>
       </c>
@@ -7520,7 +7549,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="74" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:20">
       <c r="B74" s="41" t="s">
         <v>2</v>
       </c>
@@ -7577,7 +7606,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="75" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:20">
       <c r="B75" s="33" t="s">
         <v>2</v>
       </c>
@@ -7634,7 +7663,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="76" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:20">
       <c r="B76" s="33" t="s">
         <v>2</v>
       </c>
@@ -7691,7 +7720,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="77" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:20">
       <c r="B77" s="34" t="s">
         <v>2</v>
       </c>
@@ -7748,7 +7777,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="78" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:20">
       <c r="B78" s="34" t="s">
         <v>2</v>
       </c>
@@ -7805,7 +7834,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="79" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:20">
       <c r="B79" s="34" t="s">
         <v>2</v>
       </c>
@@ -7862,7 +7891,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="80" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:20">
       <c r="B80" s="34" t="s">
         <v>2</v>
       </c>
@@ -7919,8 +7948,8 @@
         <v>629</v>
       </c>
     </row>
-    <row r="81" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="82" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:17" ht="15.75" thickBot="1"/>
+    <row r="82" spans="2:17" ht="23.25">
       <c r="B82" s="1" t="s">
         <v>368</v>
       </c>
@@ -7940,7 +7969,7 @@
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
     </row>
-    <row r="84" spans="2:17" ht="135" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:17" ht="135">
       <c r="B84" s="20" t="s">
         <v>369</v>
       </c>
@@ -7983,7 +8012,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:17">
       <c r="B85" s="23" t="s">
         <v>2</v>
       </c>
@@ -8022,7 +8051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:17">
       <c r="B86" s="23" t="s">
         <v>2</v>
       </c>
@@ -8063,7 +8092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:17">
       <c r="B87" s="26" t="s">
         <v>2</v>
       </c>
@@ -8104,7 +8133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:17">
       <c r="B88" s="26" t="s">
         <v>2</v>
       </c>
@@ -8145,7 +8174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:17">
       <c r="B89" s="26" t="s">
         <v>2</v>
       </c>
@@ -8180,7 +8209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:17">
       <c r="B90" s="26" t="s">
         <v>2</v>
       </c>
@@ -8221,8 +8250,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="92" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:17" ht="15.75" thickBot="1"/>
+    <row r="92" spans="2:17" ht="23.25">
       <c r="B92" s="1" t="s">
         <v>387</v>
       </c>
@@ -8239,11 +8268,11 @@
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
     </row>
-    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:17">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
     </row>
-    <row r="94" spans="2:17" ht="123" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:17" ht="123">
       <c r="B94" s="3" t="s">
         <v>388</v>
       </c>
@@ -8260,7 +8289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:17">
       <c r="B95" s="12" t="s">
         <v>2</v>
       </c>
@@ -8277,7 +8306,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:17">
       <c r="B96" s="17" t="s">
         <v>2</v>
       </c>
@@ -8294,7 +8323,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:6">
       <c r="B97" s="17" t="s">
         <v>2</v>
       </c>
@@ -8311,7 +8340,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:6">
       <c r="B98" s="17" t="s">
         <v>2</v>
       </c>
@@ -8328,7 +8357,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:6">
       <c r="B99" s="17" t="s">
         <v>2</v>
       </c>
@@ -8345,7 +8374,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:6">
       <c r="B100" s="17" t="s">
         <v>2</v>
       </c>
@@ -8362,7 +8391,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:6">
       <c r="B101" s="17" t="s">
         <v>2</v>
       </c>
@@ -8377,6 +8406,23 @@
       </c>
       <c r="F101" s="28" t="s">
         <v>395</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6">
+      <c r="B102" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C102" s="43" t="s">
+        <v>635</v>
+      </c>
+      <c r="D102" s="18">
+        <v>7</v>
+      </c>
+      <c r="E102" s="19" t="s">
+        <v>636</v>
+      </c>
+      <c r="F102" s="44" t="s">
+        <v>637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>